<commit_message>
toolbar and actions popup
</commit_message>
<xml_diff>
--- a/public/images/Исходники/рыбы.xlsx
+++ b/public/images/Исходники/рыбы.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bodem\fish\public\images\Исходники\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A3DE41-8934-44CF-B9B0-08D348C0AAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED24277-BC44-455F-984F-5DB274143F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Размер</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>s-barrel</t>
+  </si>
+  <si>
+    <t>H экрана</t>
+  </si>
+  <si>
+    <t>% H экрана</t>
   </si>
 </sst>
 </file>
@@ -871,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -884,7 +890,7 @@
     <col min="7" max="7" width="12.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -910,8 +916,14 @@
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>20</v>
       </c>
@@ -939,8 +951,19 @@
       <c r="I2">
         <v>5</v>
       </c>
+      <c r="J2">
+        <v>603</v>
+      </c>
+      <c r="K2">
+        <f>B2/J$2</f>
+        <v>3.316749585406302E-2</v>
+      </c>
+      <c r="L2" s="7">
+        <f>K2*1080</f>
+        <v>35.820895522388064</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>30</v>
       </c>
@@ -968,8 +991,16 @@
       <c r="I3">
         <v>3</v>
       </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="3">B3/J$2</f>
+        <v>4.975124378109453E-2</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:L10" si="4">K3*1080</f>
+        <v>53.731343283582092</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>40</v>
       </c>
@@ -997,8 +1028,16 @@
       <c r="I4">
         <v>4</v>
       </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>6.633499170812604E-2</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="4"/>
+        <v>71.641791044776127</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>60</v>
       </c>
@@ -1026,8 +1065,16 @@
       <c r="I5">
         <v>2</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>9.950248756218906E-2</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="4"/>
+        <v>107.46268656716418</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>70</v>
       </c>
@@ -1055,8 +1102,16 @@
       <c r="I6">
         <v>3</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>0.11608623548922056</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="4"/>
+        <v>125.3731343283582</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>80</v>
       </c>
@@ -1084,8 +1139,16 @@
       <c r="I7">
         <v>4</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>0.13266998341625208</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="4"/>
+        <v>143.28358208955225</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>100</v>
       </c>
@@ -1113,8 +1176,16 @@
       <c r="I8">
         <v>5</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>0.16583747927031509</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="4"/>
+        <v>179.1044776119403</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>120</v>
       </c>
@@ -1142,8 +1213,16 @@
       <c r="I9">
         <v>4</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>0.19900497512437812</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="4"/>
+        <v>214.92537313432837</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>110</v>
       </c>
@@ -1170,6 +1249,14 @@
       </c>
       <c r="I10">
         <v>7</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>0.1824212271973466</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="4"/>
+        <v>197.01492537313433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>